<commit_message>
Updated timesheet for final work
</commit_message>
<xml_diff>
--- a/Timesheets/Aidan Timesheet.xlsx
+++ b/Timesheets/Aidan Timesheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mudki\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAE0925D-B995-482A-946A-173D6FA53143}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{578C56E8-D4C7-479F-83D3-CE32C0E7DE58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,13 +16,26 @@
     <sheet name="Aidan" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
   <fileRecoveryPr repairLoad="1"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="40">
   <si>
     <t>Date</t>
   </si>
@@ -33,43 +46,10 @@
     <t>Time End</t>
   </si>
   <si>
-    <t>Total Time</t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
-    <t>1.5 h</t>
-  </si>
-  <si>
-    <t>3.5 h</t>
-  </si>
-  <si>
-    <t>2.5 h</t>
-  </si>
-  <si>
     <t>12:15:AM</t>
-  </si>
-  <si>
-    <t>4.75 h</t>
-  </si>
-  <si>
-    <t>2 h</t>
-  </si>
-  <si>
-    <t>3.75 h</t>
-  </si>
-  <si>
-    <t>4.5 h</t>
-  </si>
-  <si>
-    <t>1.75 h</t>
-  </si>
-  <si>
-    <t>5 h</t>
-  </si>
-  <si>
-    <t>10 h</t>
   </si>
   <si>
     <t>Folium research</t>
@@ -99,22 +79,13 @@
     <t>Working on icons + WSL/Ubuntu packaging for project on local device</t>
   </si>
   <si>
-    <t>9 h</t>
-  </si>
-  <si>
     <t>Prototype presentation slidedeck completion + fixing WSL and computer issues</t>
   </si>
   <si>
     <t>Trying to fix computer running code issues again</t>
   </si>
   <si>
-    <t>0.5 h</t>
-  </si>
-  <si>
     <t>Still trying to fix computer not being able to run code :(</t>
-  </si>
-  <si>
-    <t>1 h</t>
   </si>
   <si>
     <t>Computer can finally run code + minor bug fixes</t>
@@ -127,9 +98,6 @@
   </si>
   <si>
     <t>Instructions UI coding</t>
-  </si>
-  <si>
-    <t>4 h</t>
   </si>
   <si>
     <t>Instructions UI coding continued + more research</t>
@@ -164,6 +132,30 @@
   <si>
     <t>Back to changing heatmap rendering + instruction touch-ups</t>
   </si>
+  <si>
+    <t>Quick research on heatmap rendering before reflection</t>
+  </si>
+  <si>
+    <t>Finshing heatmap rendering change + bug fixes</t>
+  </si>
+  <si>
+    <t>Minor bug fixes</t>
+  </si>
+  <si>
+    <t>Final bug fixes and polishing + presentation</t>
+  </si>
+  <si>
+    <t>Total Time (Hours)</t>
+  </si>
+  <si>
+    <t>More polishing</t>
+  </si>
+  <si>
+    <t>Presentation and submission</t>
+  </si>
+  <si>
+    <t>Final presentation touch-ups</t>
+  </si>
 </sst>
 </file>
 
@@ -197,7 +189,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -219,6 +211,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -280,7 +278,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="19" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -308,10 +306,17 @@
     <xf numFmtId="18" fontId="2" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="46" fontId="3" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="46" fontId="1" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="2" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="3" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="1" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="19" fontId="1" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -533,11 +538,12 @@
   <dimension ref="A1:E1000"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="4" max="4" width="16.6640625" customWidth="1"/>
     <col min="5" max="5" width="66.44140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -552,10 +558,10 @@
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>3</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
@@ -568,11 +574,11 @@
       <c r="C2" s="10">
         <v>0.70833333333333337</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="17">
+        <v>1.5</v>
+      </c>
+      <c r="E2" s="11" t="s">
         <v>5</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
@@ -585,11 +591,11 @@
       <c r="C3" s="10">
         <v>0.72916666666666663</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="17">
+        <v>3.5</v>
+      </c>
+      <c r="E3" s="11" t="s">
         <v>6</v>
-      </c>
-      <c r="E3" s="11" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
@@ -602,11 +608,11 @@
       <c r="C4" s="10">
         <v>0.97916666666666663</v>
       </c>
-      <c r="D4" s="11" t="s">
-        <v>7</v>
+      <c r="D4" s="17">
+        <v>2.5</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
@@ -617,13 +623,13 @@
         <v>0.8125</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="11" t="s">
-        <v>9</v>
+        <v>4</v>
+      </c>
+      <c r="D5" s="17">
+        <v>4.75</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
@@ -636,11 +642,11 @@
       <c r="C6" s="10">
         <v>0.82291666666666663</v>
       </c>
-      <c r="D6" s="11" t="s">
-        <v>10</v>
+      <c r="D6" s="17">
+        <v>2</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
@@ -653,11 +659,11 @@
       <c r="C7" s="10">
         <v>0.85416666666666663</v>
       </c>
-      <c r="D7" s="11" t="s">
-        <v>11</v>
+      <c r="D7" s="17">
+        <v>3.75</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
@@ -670,11 +676,11 @@
       <c r="C8" s="10">
         <v>0</v>
       </c>
-      <c r="D8" s="11" t="s">
-        <v>12</v>
+      <c r="D8" s="17">
+        <v>4.5</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
@@ -687,11 +693,11 @@
       <c r="C9" s="10">
         <v>0.96875</v>
       </c>
-      <c r="D9" s="11" t="s">
-        <v>13</v>
+      <c r="D9" s="17">
+        <v>1.75</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
@@ -704,11 +710,11 @@
       <c r="C10" s="10">
         <v>0</v>
       </c>
-      <c r="D10" s="11" t="s">
-        <v>6</v>
+      <c r="D10" s="17">
+        <v>3.5</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
@@ -721,11 +727,11 @@
       <c r="C11" s="10">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="D11" s="11" t="s">
-        <v>14</v>
+      <c r="D11" s="17">
+        <v>5</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
@@ -738,11 +744,11 @@
       <c r="C12" s="10">
         <v>0</v>
       </c>
-      <c r="D12" s="11" t="s">
-        <v>15</v>
+      <c r="D12" s="17">
+        <v>10</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
@@ -755,11 +761,11 @@
       <c r="C13" s="14">
         <v>0.45833333333333331</v>
       </c>
-      <c r="D13" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="E13" s="18" t="s">
-        <v>26</v>
+      <c r="D13" s="18">
+        <v>9</v>
+      </c>
+      <c r="E13" s="16" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
@@ -772,11 +778,11 @@
       <c r="C14" s="14">
         <v>0.56944444444444442</v>
       </c>
-      <c r="D14" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="E14" s="16" t="s">
-        <v>27</v>
+      <c r="D14" s="19">
+        <v>0.5</v>
+      </c>
+      <c r="E14" s="15" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
@@ -789,11 +795,11 @@
       <c r="C15" s="14">
         <v>0.875</v>
       </c>
-      <c r="D15" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="E15" s="16" t="s">
-        <v>29</v>
+      <c r="D15" s="19">
+        <v>2</v>
+      </c>
+      <c r="E15" s="15" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
@@ -806,11 +812,11 @@
       <c r="C16" s="14">
         <v>0.95833333333333337</v>
       </c>
-      <c r="D16" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="E16" s="16" t="s">
-        <v>38</v>
+      <c r="D16" s="19">
+        <v>1</v>
+      </c>
+      <c r="E16" s="15" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
@@ -823,11 +829,11 @@
       <c r="C17" s="14">
         <v>0</v>
       </c>
-      <c r="D17" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="E17" s="18" t="s">
-        <v>31</v>
+      <c r="D17" s="18">
+        <v>2.5</v>
+      </c>
+      <c r="E17" s="16" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
@@ -840,11 +846,11 @@
       <c r="C18" s="14">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="D18" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="E18" s="18" t="s">
-        <v>32</v>
+      <c r="D18" s="18">
+        <v>1</v>
+      </c>
+      <c r="E18" s="16" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
@@ -857,11 +863,11 @@
       <c r="C19" s="14">
         <v>0.83333333333333337</v>
       </c>
-      <c r="D19" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="E19" s="18" t="s">
-        <v>33</v>
+      <c r="D19" s="18">
+        <v>1.5</v>
+      </c>
+      <c r="E19" s="16" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
@@ -874,11 +880,11 @@
       <c r="C20" s="14">
         <v>0.95833333333333337</v>
       </c>
-      <c r="D20" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="E20" s="18" t="s">
-        <v>34</v>
+      <c r="D20" s="18">
+        <v>1.75</v>
+      </c>
+      <c r="E20" s="16" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
@@ -891,11 +897,11 @@
       <c r="C21" s="14">
         <v>0.95833333333333337</v>
       </c>
-      <c r="D21" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="E21" s="18" t="s">
-        <v>36</v>
+      <c r="D21" s="18">
+        <v>4</v>
+      </c>
+      <c r="E21" s="16" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
@@ -908,11 +914,11 @@
       <c r="C22" s="14">
         <v>0.45833333333333331</v>
       </c>
-      <c r="D22" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="E22" s="18" t="s">
-        <v>37</v>
+      <c r="D22" s="18">
+        <v>1.5</v>
+      </c>
+      <c r="E22" s="16" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
@@ -925,11 +931,11 @@
       <c r="C23" s="14">
         <v>0.70833333333333337</v>
       </c>
-      <c r="D23" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="E23" s="18" t="s">
-        <v>39</v>
+      <c r="D23" s="18">
+        <v>0.5</v>
+      </c>
+      <c r="E23" s="16" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
@@ -942,11 +948,11 @@
       <c r="C24" s="14">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="D24" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="E24" s="18" t="s">
-        <v>40</v>
+      <c r="D24" s="18">
+        <v>0.5</v>
+      </c>
+      <c r="E24" s="16" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
@@ -959,11 +965,11 @@
       <c r="C25" s="14">
         <v>0.84375</v>
       </c>
-      <c r="D25" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="E25" s="18" t="s">
-        <v>41</v>
+      <c r="D25" s="18">
+        <v>1.75</v>
+      </c>
+      <c r="E25" s="16" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
@@ -971,16 +977,16 @@
         <v>45126</v>
       </c>
       <c r="B26" s="14">
-        <v>0.9375</v>
+        <v>0.92708333333333337</v>
       </c>
       <c r="C26" s="14">
         <v>1.0416666666666666E-2</v>
       </c>
-      <c r="D26" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="E26" s="18" t="s">
-        <v>42</v>
+      <c r="D26" s="18">
+        <v>2</v>
+      </c>
+      <c r="E26" s="16" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
@@ -993,11 +999,11 @@
       <c r="C27" s="14">
         <v>0.44791666666666669</v>
       </c>
-      <c r="D27" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="E27" s="18" t="s">
-        <v>43</v>
+      <c r="D27" s="18">
+        <v>1.5</v>
+      </c>
+      <c r="E27" s="16" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
@@ -1010,11 +1016,11 @@
       <c r="C28" s="14">
         <v>0.75</v>
       </c>
-      <c r="D28" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="E28" s="18" t="s">
-        <v>44</v>
+      <c r="D28" s="18">
+        <v>1</v>
+      </c>
+      <c r="E28" s="16" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
@@ -1022,16 +1028,16 @@
         <v>45127</v>
       </c>
       <c r="B29" s="14">
-        <v>0.9375</v>
+        <v>0.95833333333333337</v>
       </c>
       <c r="C29" s="14">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="D29" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="E29" s="16" t="s">
-        <v>45</v>
+      <c r="D29" s="19">
+        <v>3</v>
+      </c>
+      <c r="E29" s="15" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
@@ -1044,68 +1050,141 @@
       <c r="C30" s="14">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="D30" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="E30" s="16" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A31" s="5"/>
-      <c r="B31" s="6"/>
-      <c r="C31" s="6"/>
-      <c r="D31" s="7"/>
-      <c r="E31" s="8"/>
-    </row>
-    <row r="32" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A32" s="5"/>
-      <c r="B32" s="6"/>
-      <c r="C32" s="6"/>
-      <c r="D32" s="7"/>
-      <c r="E32" s="8"/>
-    </row>
-    <row r="33" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A33" s="5"/>
-      <c r="B33" s="6"/>
-      <c r="C33" s="6"/>
-      <c r="D33" s="7"/>
-      <c r="E33" s="8"/>
-    </row>
-    <row r="34" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A34" s="5"/>
-      <c r="B34" s="6"/>
-      <c r="C34" s="6"/>
-      <c r="D34" s="7"/>
-      <c r="E34" s="8"/>
-    </row>
-    <row r="35" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A35" s="5"/>
-      <c r="B35" s="6"/>
-      <c r="C35" s="6"/>
-      <c r="D35" s="7"/>
-      <c r="E35" s="8"/>
-    </row>
-    <row r="36" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A36" s="5"/>
-      <c r="B36" s="6"/>
-      <c r="C36" s="6"/>
-      <c r="D36" s="7"/>
-      <c r="E36" s="8"/>
-    </row>
-    <row r="37" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A37" s="5"/>
-      <c r="B37" s="6"/>
-      <c r="C37" s="6"/>
-      <c r="D37" s="7"/>
-      <c r="E37" s="8"/>
+      <c r="D30" s="19">
+        <v>2</v>
+      </c>
+      <c r="E30" s="15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="13">
+        <v>45130</v>
+      </c>
+      <c r="B31" s="14">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="C31" s="14">
+        <v>0.9375</v>
+      </c>
+      <c r="D31" s="19">
+        <v>0.5</v>
+      </c>
+      <c r="E31" s="15" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="13">
+        <v>45131</v>
+      </c>
+      <c r="B32" s="14">
+        <v>0.625</v>
+      </c>
+      <c r="C32" s="14">
+        <v>0.875</v>
+      </c>
+      <c r="D32" s="19">
+        <v>6</v>
+      </c>
+      <c r="E32" s="15" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="13">
+        <v>45132</v>
+      </c>
+      <c r="B33" s="14">
+        <v>0.4375</v>
+      </c>
+      <c r="C33" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="D33" s="19">
+        <v>1.5</v>
+      </c>
+      <c r="E33" s="15" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="13">
+        <v>45133</v>
+      </c>
+      <c r="B34" s="14">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="C34" s="14">
+        <v>0.625</v>
+      </c>
+      <c r="D34" s="19">
+        <v>4</v>
+      </c>
+      <c r="E34" s="15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="13">
+        <v>45133</v>
+      </c>
+      <c r="B35" s="14">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="C35" s="14">
+        <v>0.875</v>
+      </c>
+      <c r="D35" s="19">
+        <v>5</v>
+      </c>
+      <c r="E35" s="15" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="13">
+        <v>45133</v>
+      </c>
+      <c r="B36" s="14">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="C36" s="14">
+        <v>0.10416666666666667</v>
+      </c>
+      <c r="D36" s="19">
+        <v>4.5</v>
+      </c>
+      <c r="E36" s="15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="13">
+        <v>45134</v>
+      </c>
+      <c r="B37" s="14">
+        <v>0.34375</v>
+      </c>
+      <c r="C37" s="14">
+        <v>0.40625</v>
+      </c>
+      <c r="D37" s="19">
+        <v>1.5</v>
+      </c>
+      <c r="E37" s="15" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="38" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A38" s="5"/>
-      <c r="B38" s="6"/>
-      <c r="C38" s="6"/>
-      <c r="D38" s="7"/>
-      <c r="E38" s="8"/>
+      <c r="A38" s="21"/>
+      <c r="B38" s="22"/>
+      <c r="C38" s="22"/>
+      <c r="D38" s="20">
+        <f>SUM(D2:D37)</f>
+        <v>102.75</v>
+      </c>
+      <c r="E38" s="23"/>
     </row>
     <row r="39" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A39" s="5"/>

</xml_diff>